<commit_message>
change to explicit format
</commit_message>
<xml_diff>
--- a/inst/docs/example-dose-response-ec50-explicit.xlsx
+++ b/inst/docs/example-dose-response-ec50-explicit.xlsx
@@ -2006,7 +2006,7 @@
         <v>0.4148146</v>
       </c>
       <c r="G10" s="10">
-        <v>0.737799</v>
+        <v>-0.737799</v>
       </c>
       <c r="H10" t="s" s="10">
         <v>26</v>
@@ -2032,7 +2032,7 @@
         <v>0.5250468</v>
       </c>
       <c r="G11" s="10">
-        <v>0.986075</v>
+        <v>-0.986075</v>
       </c>
       <c r="H11" t="s" s="10">
         <v>26</v>
@@ -2058,7 +2058,7 @@
         <v>0.5623789</v>
       </c>
       <c r="G12" s="10">
-        <v>0.644935</v>
+        <v>-0.644935</v>
       </c>
       <c r="H12" t="s" s="10">
         <v>26</v>
@@ -2084,7 +2084,7 @@
         <v>0.9412975</v>
       </c>
       <c r="G13" s="10">
-        <v>0.931874</v>
+        <v>-0.931874</v>
       </c>
       <c r="H13" t="s" s="10">
         <v>26</v>
@@ -2110,7 +2110,7 @@
         <v>0.8161421</v>
       </c>
       <c r="G14" s="10">
-        <v>0.696713</v>
+        <v>-0.696713</v>
       </c>
       <c r="H14" t="s" s="10">
         <v>26</v>
@@ -2136,7 +2136,7 @@
         <v>0.5187678</v>
       </c>
       <c r="G15" s="10">
-        <v>0.710024</v>
+        <v>-0.710024</v>
       </c>
       <c r="H15" t="s" s="10">
         <v>26</v>
@@ -2162,7 +2162,7 @@
         <v>0.5183893000000001</v>
       </c>
       <c r="G16" s="10">
-        <v>1.42318</v>
+        <v>-1.42318</v>
       </c>
       <c r="H16" t="s" s="10">
         <v>26</v>
@@ -2188,7 +2188,7 @@
         <v>0.9263555</v>
       </c>
       <c r="G17" s="10">
-        <v>1.21865</v>
+        <v>-1.21865</v>
       </c>
       <c r="H17" t="s" s="10">
         <v>26</v>
@@ -2214,7 +2214,7 @@
         <v>1.516118</v>
       </c>
       <c r="G18" s="10">
-        <v>1.03367</v>
+        <v>-1.03367</v>
       </c>
       <c r="H18" t="s" s="10">
         <v>26</v>
@@ -2240,7 +2240,7 @@
         <v>2.133698</v>
       </c>
       <c r="G19" s="10">
-        <v>1.21384</v>
+        <v>-1.21384</v>
       </c>
       <c r="H19" t="s" s="10">
         <v>26</v>
@@ -2266,7 +2266,7 @@
         <v>1.619933</v>
       </c>
       <c r="G20" s="10">
-        <v>1.28567</v>
+        <v>-1.28567</v>
       </c>
       <c r="H20" t="s" s="10">
         <v>26</v>
@@ -2292,7 +2292,7 @@
         <v>1.108601</v>
       </c>
       <c r="G21" s="10">
-        <v>0.872721</v>
+        <v>-0.872721</v>
       </c>
       <c r="H21" t="s" s="10">
         <v>26</v>

</xml_diff>